<commit_message>
Migrating back from terraform cloud
</commit_message>
<xml_diff>
--- a/Spreadsheet-ACI.xlsx
+++ b/Spreadsheet-ACI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AE0C26-290F-4733-9362-3EE5E5A16176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B68B15-03E0-4052-92B1-43E931E0F0F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3128" uniqueCount="1108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3131" uniqueCount="1109">
   <si>
     <t>Type</t>
   </si>
@@ -4123,25 +4123,28 @@
     <t>Changed Again</t>
   </si>
   <si>
-    <t>Terraform_Cloud</t>
-  </si>
-  <si>
     <t>app.terraform.io</t>
   </si>
   <si>
     <t>Organization</t>
   </si>
   <si>
-    <t>Cisco-ITS-TigerTeam</t>
-  </si>
-  <si>
-    <t>iac-ACI-DC1</t>
-  </si>
-  <si>
-    <t>iac-ACI-DC2</t>
-  </si>
-  <si>
-    <t>Workspace_Base</t>
+    <t>atr</t>
+  </si>
+  <si>
+    <t>VCS_repo</t>
+  </si>
+  <si>
+    <t>scotttyso/iac</t>
+  </si>
+  <si>
+    <t>oauth_token_id</t>
+  </si>
+  <si>
+    <t>ot-W4vwD9rw8g1hnEX6</t>
+  </si>
+  <si>
+    <t>Terraform_Destination</t>
   </si>
 </sst>
 </file>
@@ -5349,23 +5352,23 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" style="4" customWidth="1"/>
+    <col min="1" max="3" width="12.1796875" style="4" customWidth="1"/>
     <col min="4" max="4" width="37.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="4" customWidth="1"/>
     <col min="6" max="6" width="26" style="4" customWidth="1"/>
     <col min="7" max="7" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.90625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="13.26953125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="12.1796875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="25.7265625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="26.453125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="20.6328125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="15" style="4" customWidth="1"/>
     <col min="15" max="15" width="12.54296875" style="4" customWidth="1"/>
     <col min="16" max="16" width="12.453125" style="4" customWidth="1"/>
     <col min="17" max="17" width="11.81640625" style="4" customWidth="1"/>
@@ -5422,33 +5425,35 @@
         <v>678</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>1101</v>
+        <v>1108</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="H3" s="49" t="s">
+        <v>1106</v>
+      </c>
+      <c r="I3" s="49" t="s">
         <v>584</v>
       </c>
-      <c r="I3" s="49" t="s">
+      <c r="J3" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="49" t="s">
+      <c r="K3" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="49" t="s">
+      <c r="L3" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="49" t="s">
+      <c r="M3" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="49" t="s">
+      <c r="N3" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="49"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="50" t="s">
@@ -5464,25 +5469,25 @@
         <v>1093</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G4" s="104" t="s">
         <v>1105</v>
       </c>
-      <c r="H4" s="52">
+      <c r="H4" s="34" t="s">
+        <v>1107</v>
+      </c>
+      <c r="I4" s="52">
         <v>65501</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="J4" s="14" t="s">
         <v>595</v>
       </c>
-      <c r="J4" s="34" t="s">
+      <c r="K4" s="34" t="s">
         <v>590</v>
-      </c>
-      <c r="K4" s="31">
-        <v>5555555</v>
       </c>
       <c r="L4" s="31">
         <v>5555555</v>
@@ -5490,7 +5495,9 @@
       <c r="M4" s="31">
         <v>5555555</v>
       </c>
-      <c r="N4" s="31"/>
+      <c r="N4" s="31">
+        <v>5555555</v>
+      </c>
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="53" t="s">
@@ -5506,25 +5513,25 @@
         <v>1094</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>1106</v>
-      </c>
-      <c r="H5" s="55">
+        <v>1105</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>1107</v>
+      </c>
+      <c r="I5" s="55">
         <v>65502</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="J5" s="42" t="s">
         <v>596</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="K5" s="42" t="s">
         <v>591</v>
-      </c>
-      <c r="K5" s="42">
-        <v>5555555</v>
       </c>
       <c r="L5" s="42">
         <v>5555555</v>
@@ -5532,7 +5539,9 @@
       <c r="M5" s="42">
         <v>5555555</v>
       </c>
-      <c r="N5" s="20"/>
+      <c r="N5" s="42">
+        <v>5555555</v>
+      </c>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="50"/>
@@ -5886,7 +5895,7 @@
     <mergeCell ref="B18:N18"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="BGP ASN" error="BGP ASN Must be between 1 and 4294967295" sqref="D6:D15 H4:H5" xr:uid="{7F97824C-0114-4CBA-A34D-C5EE10D10460}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="BGP ASN" error="BGP ASN Must be between 1 and 4294967295" sqref="D6:D15 I4:I5" xr:uid="{7F97824C-0114-4CBA-A34D-C5EE10D10460}">
       <formula1>1</formula1>
       <formula2>4294967295</formula2>
     </dataValidation>
@@ -19249,7 +19258,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
moving away from terraform cloud for now
</commit_message>
<xml_diff>
--- a/Spreadsheet-ACI.xlsx
+++ b/Spreadsheet-ACI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B68B15-03E0-4052-92B1-43E931E0F0F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35959C10-F8AF-42EE-A725-847809FB2320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="15" r:id="rId1"/>
@@ -4033,9 +4033,6 @@
     <t>Inband</t>
   </si>
   <si>
-    <t>Access_phys</t>
-  </si>
-  <si>
     <t>dmz_Ext</t>
   </si>
   <si>
@@ -4144,7 +4141,10 @@
     <t>ot-W4vwD9rw8g1hnEX6</t>
   </si>
   <si>
-    <t>Terraform_Destination</t>
+    <t>Terraform_State_Dest</t>
+  </si>
+  <si>
+    <t>access_phys</t>
   </si>
 </sst>
 </file>
@@ -5351,16 +5351,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFD7935-0F0A-46EB-9824-225EC9CADD69}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="12.1796875" style="4" customWidth="1"/>
     <col min="4" max="4" width="37.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="4" customWidth="1"/>
-    <col min="6" max="6" width="26" style="4" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" style="4" customWidth="1"/>
     <col min="7" max="7" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.7265625" style="4" customWidth="1"/>
     <col min="9" max="9" width="9.26953125" style="4" customWidth="1"/>
@@ -5425,16 +5425,16 @@
         <v>678</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="I3" s="49" t="s">
         <v>584</v>
@@ -5466,19 +5466,19 @@
         <v>590</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G4" s="104" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="I4" s="52">
         <v>65501</v>
@@ -5510,19 +5510,19 @@
         <v>591</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="H5" s="42" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="I5" s="55">
         <v>65502</v>
@@ -6034,7 +6034,7 @@
         <v>256</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>679</v>
@@ -6087,7 +6087,7 @@
         <v>294</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>471</v>
@@ -8583,8 +8583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AG141"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T41" sqref="T41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11146,7 +11146,7 @@
       <c r="C42" s="31"/>
       <c r="D42" s="31"/>
       <c r="E42" s="31" t="s">
-        <v>1071</v>
+        <v>1108</v>
       </c>
       <c r="F42" s="33"/>
       <c r="G42" s="33"/>
@@ -11207,7 +11207,7 @@
       <c r="C43" s="20"/>
       <c r="D43" s="20"/>
       <c r="E43" s="20" t="s">
-        <v>1071</v>
+        <v>1108</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
@@ -11233,7 +11233,7 @@
         <v>87</v>
       </c>
       <c r="U43" s="20" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="V43" s="20" t="s">
         <v>540</v>
@@ -11714,10 +11714,10 @@
         <v>392</v>
       </c>
       <c r="C58" s="7" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>1077</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>1078</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>522</v>
@@ -11741,7 +11741,7 @@
         <v>501</v>
       </c>
       <c r="L58" s="7" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="M58" s="7" t="s">
         <v>534</v>
@@ -12123,7 +12123,7 @@
         <v>701</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
@@ -12163,7 +12163,7 @@
         <v>702</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
@@ -13470,10 +13470,10 @@
         <v>392</v>
       </c>
       <c r="C124" s="7" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D124" s="7" t="s">
         <v>1082</v>
-      </c>
-      <c r="D124" s="7" t="s">
-        <v>1083</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>705</v>
@@ -13491,16 +13491,16 @@
         <v>706</v>
       </c>
       <c r="J124" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="K124" s="7" t="s">
         <v>1085</v>
       </c>
-      <c r="K124" s="7" t="s">
+      <c r="L124" s="7" t="s">
         <v>1086</v>
       </c>
-      <c r="L124" s="7" t="s">
-        <v>1087</v>
-      </c>
       <c r="M124" s="7" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="N124" s="7" t="s">
         <v>710</v>
@@ -13514,7 +13514,7 @@
     </row>
     <row r="125" spans="1:20" s="65" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A125" s="31" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B125" s="31" t="s">
         <v>102</v>
@@ -13887,7 +13887,7 @@
         <v>407</v>
       </c>
       <c r="U137" s="43" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="V137" s="7" t="s">
         <v>408</v>
@@ -16993,7 +16993,7 @@
         <v>588</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>121</v>
@@ -17132,7 +17132,7 @@
         <v>589</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>121</v>
@@ -19637,7 +19637,7 @@
         <v>592</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>219</v>
@@ -19674,7 +19674,7 @@
         <v>592</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>222</v>
@@ -19773,7 +19773,7 @@
         <v>231</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="E22" s="31" t="s">
         <v>225</v>
@@ -19901,7 +19901,7 @@
         <v>14</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E28" s="33">
         <v>48</v>
@@ -21983,7 +21983,7 @@
         <v>679</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="N3" s="7"/>
       <c r="P3"/>
@@ -21991,7 +21991,7 @@
     </row>
     <row r="4" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="31" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>592</v>
@@ -22031,7 +22031,7 @@
     </row>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="20" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>588</v>
@@ -22055,7 +22055,7 @@
         <v>897</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="J5" s="20" t="s">
         <v>898</v>
@@ -22073,7 +22073,7 @@
     </row>
     <row r="6" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="31" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>589</v>
@@ -22097,7 +22097,7 @@
         <v>897</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="J6" s="31" t="s">
         <v>898</v>
@@ -22115,7 +22115,7 @@
     </row>
     <row r="7" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="20" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>588</v>
@@ -22139,7 +22139,7 @@
         <v>897</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>906</v>
@@ -22157,7 +22157,7 @@
     </row>
     <row r="8" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="31" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>589</v>
@@ -22181,7 +22181,7 @@
         <v>897</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="J8" s="31" t="s">
         <v>906</v>
@@ -22314,7 +22314,7 @@
         <v>183</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>886</v>
@@ -22323,7 +22323,7 @@
         <v>184</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="N15" s="7" t="s">
         <v>882</v>
@@ -22332,7 +22332,7 @@
     </row>
     <row r="16" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="31" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>588</v>
@@ -22371,7 +22371,7 @@
     </row>
     <row r="17" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>588</v>
@@ -22410,7 +22410,7 @@
     </row>
     <row r="18" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="31" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>589</v>
@@ -22449,7 +22449,7 @@
     </row>
     <row r="19" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>589</v>
@@ -22488,7 +22488,7 @@
     </row>
     <row r="20" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="31" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B20" s="31" t="s">
         <v>588</v>
@@ -22533,7 +22533,7 @@
     </row>
     <row r="21" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>589</v>
@@ -22578,7 +22578,7 @@
     </row>
     <row r="22" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="31" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>588</v>
@@ -22617,7 +22617,7 @@
     </row>
     <row r="23" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>588</v>
@@ -22656,7 +22656,7 @@
     </row>
     <row r="24" spans="1:17" s="66" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="31" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>589</v>
@@ -22694,7 +22694,7 @@
     </row>
     <row r="25" spans="1:17" s="66" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>589</v>
@@ -23526,7 +23526,7 @@
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7" t="s">
@@ -23718,7 +23718,7 @@
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7" t="s">
@@ -23915,7 +23915,7 @@
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="7" t="s">

</xml_diff>